<commit_message>
Added Color Coded Sheet of Specs
</commit_message>
<xml_diff>
--- a/All AutoText Index2.xlsx
+++ b/All AutoText Index2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio\Documents\GitHub\SDI_Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83F0933D-F2D6-4010-B8C6-322322AC1F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE4DB155-1DE5-4C16-AD72-0065F374AFAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42360" yWindow="3540" windowWidth="29340" windowHeight="15585" xr2:uid="{9913C9D4-04A4-4B48-B591-6E761B065B25}"/>
+    <workbookView xWindow="3000" yWindow="3435" windowWidth="29340" windowHeight="15585" xr2:uid="{9913C9D4-04A4-4B48-B591-6E761B065B25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1773" uniqueCount="1238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1777" uniqueCount="1240">
   <si>
     <t>AIR CURTAIN</t>
   </si>
@@ -3739,6 +3739,12 @@
   </si>
   <si>
     <t>HOT WATER DISPENSER_Bunn_HW2 SST</t>
+  </si>
+  <si>
+    <t>BEL0095</t>
+  </si>
+  <si>
+    <t>EVAPORATOR COIL_RDT_BEL0095</t>
   </si>
 </sst>
 </file>
@@ -4133,10 +4139,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67270D1F-9252-4710-A74A-D374ABF48298}">
-  <dimension ref="A1:M458"/>
+  <dimension ref="A1:M459"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A259" sqref="A259:XFD259"/>
+    <sheetView tabSelected="1" topLeftCell="A448" workbookViewId="0">
+      <selection activeCell="K459" sqref="K459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14801,6 +14807,20 @@
         <v>1230</v>
       </c>
     </row>
+    <row r="459" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B459" t="s">
+        <v>163</v>
+      </c>
+      <c r="D459" t="s">
+        <v>164</v>
+      </c>
+      <c r="E459" s="2" t="s">
+        <v>1238</v>
+      </c>
+      <c r="K459" t="s">
+        <v>1239</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K458">
     <sortCondition ref="A2:A458"/>

</xml_diff>